<commit_message>
add bar chart with amplitude changes from sensitivity analysis, its easier using pandas
</commit_message>
<xml_diff>
--- a/data_analysis/simulations/hong_robustness.xlsx
+++ b/data_analysis/simulations/hong_robustness.xlsx
@@ -31,6 +31,9 @@
     <t>amplitude FRQn +</t>
   </si>
   <si>
+    <t>phase frq mRNA +</t>
+  </si>
+  <si>
     <t>phase wc-1 mRNA +</t>
   </si>
   <si>
@@ -52,9 +55,6 @@
     <t>phase WC-1n +</t>
   </si>
   <si>
-    <t>phase frq mRNA +</t>
-  </si>
-  <si>
     <t>amplitude WC-1n +</t>
   </si>
   <si>
@@ -94,6 +94,9 @@
     <t>amplitude FRQn -</t>
   </si>
   <si>
+    <t>phase frq mRNA -</t>
+  </si>
+  <si>
     <t>phase wc-1 mRNA -</t>
   </si>
   <si>
@@ -113,9 +116,6 @@
   </si>
   <si>
     <t>phase WC-1n -</t>
-  </si>
-  <si>
-    <t>phase frq mRNA -</t>
   </si>
   <si>
     <t>amplitude WC-1n -</t>
@@ -716,64 +716,64 @@
         <v>42</v>
       </c>
       <c r="B2">
-        <v>-0.09727626459142724</v>
+        <v>-0.0972762645914272</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-8.973108320345931</v>
+        <v>-8.9731335067334</v>
       </c>
       <c r="E2">
-        <v>-0.2172390085436336</v>
+        <v>-0.217239008543634</v>
       </c>
       <c r="F2">
-        <v>-29.24858245383613</v>
+        <v>-29.2485457388351</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>-0.3368826068547326</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>-6.762070642971146</v>
+        <v>-0.336882606854733</v>
       </c>
       <c r="J2">
-        <v>-0.06985679357317474</v>
-      </c>
-      <c r="L2">
-        <v>0.8769209953659379</v>
+        <v>-6.76206385780949</v>
+      </c>
+      <c r="K2">
+        <v>-0.0698567935731747</v>
       </c>
       <c r="M2">
-        <v>-2.422242473802317</v>
+        <v>0.876920995365938</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>-2.42224247380232</v>
       </c>
       <c r="O2">
-        <v>-5.683974444524453</v>
+        <v>-5.68396344262495</v>
       </c>
       <c r="P2">
-        <v>-0.06985679357317474</v>
+        <v>-0.0698567935731747</v>
       </c>
       <c r="Q2">
-        <v>-6.745183977630767</v>
+        <v>-6.74518078029747</v>
       </c>
       <c r="R2">
         <v>-0.104748603351963</v>
       </c>
       <c r="S2">
-        <v>-0.06985679357317474</v>
+        <v>-0.0698567935731747</v>
       </c>
       <c r="T2">
-        <v>-6.823006299524266</v>
+        <v>-6.8229976182306</v>
       </c>
       <c r="U2">
-        <v>-0.09727626459142724</v>
+        <v>-0.0972762645914272</v>
       </c>
       <c r="V2">
-        <v>0.9287667410312959</v>
+        <v>0.928766741031296</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -782,43 +782,43 @@
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>7.715369293936019</v>
+        <v>7.71532661819974</v>
       </c>
       <c r="Z2">
-        <v>-1.004304160688672</v>
+        <v>-1.00430416068867</v>
       </c>
       <c r="AA2">
-        <v>41.42008067882966</v>
+        <v>41.4201287571302</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>-2.032520325203249</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>5.553556039726612</v>
+        <v>-2.03252032520325</v>
       </c>
       <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>-2.016129032258061</v>
+        <v>5.55356182731081</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>2.517162471395872</v>
+        <v>-2.01612903225806</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>2.51716247139587</v>
       </c>
       <c r="AJ2">
-        <v>3.835255759754884</v>
+        <v>3.83526466865618</v>
       </c>
       <c r="AK2">
         <v>0</v>
       </c>
       <c r="AL2">
-        <v>5.541035789957514</v>
+        <v>5.54103275626348</v>
       </c>
       <c r="AM2">
         <v>0</v>
@@ -827,13 +827,13 @@
         <v>0</v>
       </c>
       <c r="AO2">
-        <v>5.658629864401217</v>
+        <v>5.65863750760554</v>
       </c>
       <c r="AP2">
-        <v>-0.03242542153047575</v>
+        <v>-0.0324254215304757</v>
       </c>
       <c r="AQ2">
-        <v>-3.292181069958857</v>
+        <v>-3.29218106995886</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -841,124 +841,124 @@
         <v>43</v>
       </c>
       <c r="B3">
-        <v>-0.06485084306096763</v>
+        <v>-0.0648508430609676</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>10.24045803391182</v>
+        <v>10.2404240215497</v>
       </c>
       <c r="E3">
-        <v>-0.3956258578494009</v>
+        <v>-0.395625857849401</v>
       </c>
       <c r="F3">
-        <v>1.336453530773355</v>
+        <v>1.33646885005184</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>-1.184997699033595</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.15447461617053</v>
+        <v>-1.18499769903359</v>
       </c>
       <c r="J3">
-        <v>-0.03492839678657931</v>
-      </c>
-      <c r="L3">
+        <v>0.154476656406807</v>
+      </c>
+      <c r="K3">
+        <v>-0.0349283967865793</v>
+      </c>
+      <c r="M3">
         <v>-0.77179279096503</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.293874375015767</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
       <c r="O3">
-        <v>-0.4086077242363041</v>
+        <v>-0.408602835550364</v>
       </c>
       <c r="P3">
-        <v>-0.03492839678657931</v>
+        <v>-0.0349283967865793</v>
       </c>
       <c r="Q3">
-        <v>0.1744635244018827</v>
+        <v>0.174453011570957</v>
       </c>
       <c r="R3">
-        <v>-0.06983240223463663</v>
+        <v>-0.0698324022346366</v>
       </c>
       <c r="S3">
-        <v>-0.03492839678657931</v>
+        <v>-0.0349283967865793</v>
       </c>
       <c r="T3">
-        <v>0.1808254205543319</v>
+        <v>0.180828824274609</v>
       </c>
       <c r="U3">
-        <v>-0.06485084306096763</v>
+        <v>-0.0648508430609676</v>
       </c>
       <c r="V3">
-        <v>-0.7537392194586071</v>
+        <v>-0.753739219458607</v>
       </c>
       <c r="W3">
-        <v>0.03242542153047575</v>
+        <v>0.0324254215304757</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>-10.2168702096977</v>
+        <v>-10.2168956223395</v>
       </c>
       <c r="Z3">
-        <v>-0.2131798958889043</v>
+        <v>-0.213179895888904</v>
       </c>
       <c r="AA3">
-        <v>-1.371044129844301</v>
+        <v>-1.37097882722279</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>-0.8822486130620579</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>-0.1712604478826214</v>
+        <v>-0.882248613062058</v>
       </c>
       <c r="AE3">
-        <v>0.06985679357319088</v>
-      </c>
-      <c r="AG3">
-        <v>-0.4727523503912605</v>
+        <v>-0.171247934116856</v>
+      </c>
+      <c r="AF3">
+        <v>0.0698567935731909</v>
       </c>
       <c r="AH3">
-        <v>0.4251026410363719</v>
+        <v>-0.47275235039126</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>0.425102641036372</v>
       </c>
       <c r="AJ3">
-        <v>0.3913355680381148</v>
+        <v>0.39135105831</v>
       </c>
       <c r="AK3">
-        <v>0.06985679357319088</v>
+        <v>0.0698567935731909</v>
       </c>
       <c r="AL3">
-        <v>-0.1916404381131591</v>
+        <v>-0.191640223489075</v>
       </c>
       <c r="AM3">
-        <v>0.03491620111732637</v>
+        <v>0.0349162011173264</v>
       </c>
       <c r="AN3">
-        <v>0.06985679357319088</v>
+        <v>0.0698567935731909</v>
       </c>
       <c r="AO3">
-        <v>-0.197596033978589</v>
+        <v>-0.197585936927983</v>
       </c>
       <c r="AP3">
-        <v>0.03242542153047575</v>
+        <v>0.0324254215304757</v>
       </c>
       <c r="AQ3">
-        <v>-0.4462830097889298</v>
+        <v>-0.44628300978893</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -966,124 +966,124 @@
         <v>44</v>
       </c>
       <c r="B4">
-        <v>-1.459143968871586</v>
+        <v>-1.45914396887159</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>39.0572242984505</v>
+        <v>39.0571801905265</v>
       </c>
       <c r="E4">
         <v>-3.05692698375485</v>
       </c>
       <c r="F4">
-        <v>271.3809447901224</v>
+        <v>271.381169249206</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>-7.205391820035612</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>27.02694841258704</v>
+        <v>-7.20539182003561</v>
       </c>
       <c r="J4">
-        <v>-1.434559153734826</v>
-      </c>
-      <c r="L4">
-        <v>-6.317357397668204</v>
+        <v>27.0269587484251</v>
+      </c>
+      <c r="K4">
+        <v>-1.43455915373483</v>
       </c>
       <c r="M4">
-        <v>1.016307453900198</v>
+        <v>-6.3173573976682</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1.0163074539002</v>
       </c>
       <c r="O4">
-        <v>14.62985745972192</v>
+        <v>14.6298712297113</v>
       </c>
       <c r="P4">
-        <v>-1.434559153734826</v>
+        <v>-1.43455915373483</v>
       </c>
       <c r="Q4">
-        <v>27.80409474575355</v>
+        <v>27.8041007456776</v>
       </c>
       <c r="R4">
-        <v>-1.501396648044695</v>
+        <v>-1.5013966480447</v>
       </c>
       <c r="S4">
-        <v>-1.434559153734826</v>
+        <v>-1.43455915373483</v>
       </c>
       <c r="T4">
-        <v>28.31436880468601</v>
+        <v>28.3143826745299</v>
       </c>
       <c r="U4">
-        <v>-1.459143968871586</v>
+        <v>-1.45914396887159</v>
       </c>
       <c r="V4">
-        <v>-10.17398902703562</v>
+        <v>-10.1739890270356</v>
       </c>
       <c r="W4">
-        <v>1.092487279257695</v>
+        <v>1.0924872792577</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>-84.14984482085512</v>
+        <v>-84.1498501619857</v>
       </c>
       <c r="Z4">
-        <v>117.3432094481016</v>
+        <v>117.343209448102</v>
       </c>
       <c r="AA4">
-        <v>-92.83236908757056</v>
+        <v>-92.8323621359666</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>4.631222660774323</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <v>-81.60873719382636</v>
+        <v>4.63122266077432</v>
       </c>
       <c r="AE4">
-        <v>1.012923506811042</v>
-      </c>
-      <c r="AG4">
-        <v>4.984969660464918</v>
+        <v>-81.6087193157958</v>
+      </c>
+      <c r="AF4">
+        <v>1.01292350681104</v>
       </c>
       <c r="AH4">
-        <v>-21.90580077135845</v>
+        <v>4.98496966046492</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>-21.9058007713585</v>
       </c>
       <c r="AJ4">
-        <v>-79.9563742473193</v>
+        <v>-79.9563527041009</v>
       </c>
       <c r="AK4">
-        <v>0.9979541939024963</v>
+        <v>0.997954193902496</v>
       </c>
       <c r="AL4">
-        <v>-81.12004412622726</v>
+        <v>-81.1200298271313</v>
       </c>
       <c r="AM4">
-        <v>0.9776536312849128</v>
+        <v>0.977653631284913</v>
       </c>
       <c r="AN4">
-        <v>1.012923506811042</v>
+        <v>1.01292350681104</v>
       </c>
       <c r="AO4">
-        <v>-81.1322919600612</v>
+        <v>-81.1322732454322</v>
       </c>
       <c r="AP4">
-        <v>0.9877282250823072</v>
+        <v>0.987728225082307</v>
       </c>
       <c r="AQ4">
-        <v>10.85042319097951</v>
+        <v>10.8504231909795</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -1091,64 +1091,64 @@
         <v>45</v>
       </c>
       <c r="B5">
-        <v>-1.134889753566796</v>
+        <v>-1.1348897535668</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>30.00513180639421</v>
+        <v>30.0050904384103</v>
       </c>
       <c r="E5">
-        <v>-0.7558760940945398</v>
+        <v>-0.75587609409454</v>
       </c>
       <c r="F5">
-        <v>132.2572347103201</v>
+        <v>132.257493756363</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>-3.810125670951692</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>10.00705924048606</v>
+        <v>-3.81012567095169</v>
       </c>
       <c r="J5">
-        <v>-1.110224040716523</v>
-      </c>
-      <c r="L5">
-        <v>-3.770344912337515</v>
+        <v>10.0070748832365</v>
+      </c>
+      <c r="K5">
+        <v>-1.11022404071652</v>
       </c>
       <c r="M5">
-        <v>-1.861059596386415</v>
+        <v>-3.77034491233752</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>-1.86105959638641</v>
       </c>
       <c r="O5">
-        <v>3.198397337373229</v>
+        <v>3.19841757328054</v>
       </c>
       <c r="P5">
-        <v>-1.117708697170796</v>
+        <v>-1.1177086971708</v>
       </c>
       <c r="Q5">
-        <v>10.6772099330587</v>
+        <v>10.6772104155187</v>
       </c>
       <c r="R5">
         <v>-1.14475259377494</v>
       </c>
       <c r="S5">
-        <v>-1.110224040716523</v>
+        <v>-1.11022404071652</v>
       </c>
       <c r="T5">
-        <v>10.9592822460917</v>
+        <v>10.9593026389552</v>
       </c>
       <c r="U5">
-        <v>-1.134889753566796</v>
+        <v>-1.1348897535668</v>
       </c>
       <c r="V5">
-        <v>-5.918888813098192</v>
+        <v>-5.91888881309819</v>
       </c>
       <c r="W5">
         <v>-0.291828793774314</v>
@@ -1157,58 +1157,58 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>-60.01296325795126</v>
+        <v>-60.0129718829964</v>
       </c>
       <c r="Z5">
-        <v>0.6384580453709556</v>
+        <v>0.638458045370956</v>
       </c>
       <c r="AA5">
-        <v>-77.77370920095599</v>
+        <v>-77.7736897638741</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>4.800992473835023</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>-48.53778205816629</v>
+        <v>4.80099247383502</v>
       </c>
       <c r="AE5">
+        <v>-48.5377599802936</v>
+      </c>
+      <c r="AF5">
         <v>-0.279427174292699</v>
       </c>
-      <c r="AG5">
-        <v>4.323767018812497</v>
-      </c>
       <c r="AH5">
-        <v>-11.41195512641626</v>
+        <v>4.3237670188125</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>-11.4119551264163</v>
       </c>
       <c r="AJ5">
-        <v>-46.54820564262717</v>
+        <v>-46.5481794876738</v>
       </c>
       <c r="AK5">
-        <v>-0.3492839678658737</v>
+        <v>-0.349283967865874</v>
       </c>
       <c r="AL5">
-        <v>-48.61735991470743</v>
+        <v>-48.6173391878645</v>
       </c>
       <c r="AM5">
-        <v>-0.3491620111731831</v>
+        <v>-0.349162011173183</v>
       </c>
       <c r="AN5">
-        <v>-0.3143555710792783</v>
+        <v>-0.314355571079278</v>
       </c>
       <c r="AO5">
-        <v>-48.63123424300352</v>
+        <v>-48.6312100467794</v>
       </c>
       <c r="AP5">
-        <v>-0.3392197944727116</v>
+        <v>-0.339219794472712</v>
       </c>
       <c r="AQ5">
-        <v>9.022640954432584</v>
+        <v>9.02264095443258</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -1222,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.05028728003549392</v>
+        <v>0.0502670811722182</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.1387533772007958</v>
+        <v>0.138865886602737</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1237,12 +1237,12 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.02459009820916655</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+        <v>0.0246123188495124</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
       <c r="M6">
@@ -1252,13 +1252,13 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.01807683259658865</v>
+        <v>0.0181048926785239</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.02560797069216175</v>
+        <v>0.0256239677409469</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0.0257831889405698</v>
+        <v>0.0258066967161493</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1282,43 +1282,43 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>-0.0502840318924276</v>
+        <v>-0.0503302728775881</v>
       </c>
       <c r="Z6">
-        <v>-0.1434720229555296</v>
+        <v>-0.14347202295553</v>
       </c>
       <c r="AA6">
-        <v>-0.1393560094118157</v>
+        <v>-0.139270770547985</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>-0.4065040650406548</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>-0.02463887740061008</v>
+        <v>-0.406504065040655</v>
       </c>
       <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>-0.4032258064516172</v>
+        <v>-0.0246244788972855</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>0.2288329519450653</v>
+        <v>-0.403225806451617</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>0.228832951945065</v>
       </c>
       <c r="AJ6">
-        <v>-0.01815795168076673</v>
+        <v>-0.0181390767180962</v>
       </c>
       <c r="AK6">
         <v>0</v>
       </c>
       <c r="AL6">
-        <v>-0.02565936140111085</v>
+        <v>-0.0256502847767565</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="AO6">
-        <v>-0.02584838215542892</v>
+        <v>-0.025833205728962</v>
       </c>
       <c r="AP6">
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>-0.4115226337448697</v>
+        <v>-0.41152263374487</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -1341,124 +1341,124 @@
         <v>47</v>
       </c>
       <c r="B7">
-        <v>-0.6809338521400875</v>
+        <v>-0.680933852140088</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-2.401792003501376</v>
+        <v>-2.40183195181442</v>
       </c>
       <c r="E7">
-        <v>-0.3429405105666974</v>
+        <v>-0.342940510566697</v>
       </c>
       <c r="F7">
-        <v>-6.609051773990977</v>
+        <v>-6.60899872469539</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>-0.1578892455842384</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>-1.806060491380282</v>
+        <v>-0.157889245584238</v>
       </c>
       <c r="J7">
-        <v>-0.6561548824908954</v>
-      </c>
-      <c r="L7">
-        <v>0.2545996440344194</v>
+        <v>-1.8060539388896</v>
+      </c>
+      <c r="K7">
+        <v>-0.656154882490895</v>
       </c>
       <c r="M7">
-        <v>-0.2360049935339659</v>
+        <v>0.254599644034419</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>-0.236004993533966</v>
       </c>
       <c r="O7">
-        <v>-2.582440481859651</v>
+        <v>-2.58243129535983</v>
       </c>
       <c r="P7">
         <v>-0.663639538945152</v>
       </c>
       <c r="Q7">
-        <v>-2.115380086907324</v>
+        <v>-2.11538055212544</v>
       </c>
       <c r="R7">
-        <v>-0.6908419792498101</v>
+        <v>-0.69084197924981</v>
       </c>
       <c r="S7">
-        <v>-0.6561548824908954</v>
+        <v>-0.656154882490895</v>
       </c>
       <c r="T7">
-        <v>-2.093507773101169</v>
+        <v>-2.09349960042003</v>
       </c>
       <c r="U7">
-        <v>-0.6809338521400875</v>
+        <v>-0.680933852140088</v>
       </c>
       <c r="V7">
-        <v>0.2812624244045879</v>
+        <v>0.281262424404588</v>
       </c>
       <c r="W7">
-        <v>0.6809338521400714</v>
+        <v>0.680933852140071</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>2.340226662496909</v>
+        <v>2.34021525574763</v>
       </c>
       <c r="Z7">
-        <v>-0.3008733685280866</v>
+        <v>-0.300873368528087</v>
       </c>
       <c r="AA7">
-        <v>7.014388472906222</v>
+        <v>7.0145049002144</v>
       </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>-1.097405875203399</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <v>1.73454095803073</v>
+        <v>-1.0974058752034</v>
       </c>
       <c r="AE7">
-        <v>0.6985679357317637</v>
-      </c>
-      <c r="AG7">
-        <v>-0.6937218175511588</v>
+        <v>1.73455760966843</v>
+      </c>
+      <c r="AF7">
+        <v>0.698567935731764</v>
       </c>
       <c r="AH7">
-        <v>0.4600979449253337</v>
+        <v>-0.693721817551159</v>
       </c>
       <c r="AI7">
-        <v>0</v>
+        <v>0.460097944925334</v>
       </c>
       <c r="AJ7">
-        <v>2.542386615628101</v>
+        <v>2.54241004204838</v>
       </c>
       <c r="AK7">
         <v>0.733496332518343</v>
       </c>
       <c r="AL7">
-        <v>2.058534395557481</v>
+        <v>2.05854816502081</v>
       </c>
       <c r="AM7">
-        <v>0.6634078212290559</v>
+        <v>0.663407821229056</v>
       </c>
       <c r="AN7">
-        <v>0.6985679357317637</v>
+        <v>0.698567935731764</v>
       </c>
       <c r="AO7">
-        <v>2.035601763354765</v>
+        <v>2.03562194758733</v>
       </c>
       <c r="AP7">
-        <v>0.6734510625561266</v>
+        <v>0.673451062556127</v>
       </c>
       <c r="AQ7">
-        <v>-0.6590357266735981</v>
+        <v>-0.659035726673598</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -1472,43 +1472,43 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.6678417199734609</v>
+        <v>0.66782207044916</v>
       </c>
       <c r="E8">
-        <v>-0.1434720229555296</v>
+        <v>-0.14347202295553</v>
       </c>
       <c r="F8">
-        <v>-5.539573026897212</v>
+        <v>-5.53948328055364</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>-0.4065040650406548</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0.457408600157252</v>
+        <v>-0.406504065040655</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>-0.4032258064516172</v>
+        <v>0.4574253430718</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>0.4576659038901585</v>
+        <v>-0.403225806451617</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.457665903890159</v>
       </c>
       <c r="O8">
-        <v>0.6730060763588043</v>
+        <v>0.673024527230707</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0.5639342550075601</v>
+        <v>0.563944259019094</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1517,13 +1517,13 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>0.4394584951062378</v>
+        <v>0.439477433671045</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0.4115226337448445</v>
+        <v>0.411522633744845</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1532,13 +1532,13 @@
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>-0.7989650992085975</v>
+        <v>-0.799000214442468</v>
       </c>
       <c r="Z8">
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>6.404049138589077</v>
+        <v>6.4040823943989</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -1547,12 +1547,12 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>-0.5507739264889413</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
+        <v>-0.550768522645132</v>
+      </c>
+      <c r="AF8">
         <v>0</v>
       </c>
       <c r="AH8">
@@ -1562,13 +1562,13 @@
         <v>0</v>
       </c>
       <c r="AJ8">
-        <v>-0.7988124113105276</v>
+        <v>-0.798803084003268</v>
       </c>
       <c r="AK8">
         <v>0</v>
       </c>
       <c r="AL8">
-        <v>-0.6792997027588809</v>
+        <v>-0.679303505849057</v>
       </c>
       <c r="AM8">
         <v>0</v>
@@ -1577,13 +1577,13 @@
         <v>0</v>
       </c>
       <c r="AO8">
-        <v>-0.529246654433559</v>
+        <v>-0.529240630248175</v>
       </c>
       <c r="AP8">
         <v>0</v>
       </c>
       <c r="AQ8">
-        <v>-0.8230452674897143</v>
+        <v>-0.823045267489714</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -1597,13 +1597,13 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-0.08240931764976837</v>
+        <v>-0.0824089829847565</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.6621047195032406</v>
+        <v>0.662090654813</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1612,12 +1612,12 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>-0.05663361923279896</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+        <v>-0.0566367015413005</v>
+      </c>
+      <c r="K9">
         <v>0</v>
       </c>
       <c r="M9">
@@ -1627,13 +1627,13 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>-0.08251456912344489</v>
+        <v>-0.0825178556241582</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>-0.06978057316049392</v>
+        <v>-0.0697877009415544</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>-0.05449101776902995</v>
+        <v>-0.054490729309879</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1657,43 +1657,43 @@
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>0.08266953573735084</v>
+        <v>0.0826571987566559</v>
       </c>
       <c r="Z9">
-        <v>-0.1434720229555296</v>
+        <v>-0.14347202295553</v>
       </c>
       <c r="AA9">
-        <v>-0.6663022704480644</v>
+        <v>-0.666250998215201</v>
       </c>
       <c r="AB9">
         <v>0</v>
       </c>
       <c r="AC9">
-        <v>-0.4065040650406548</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <v>0.05673111435291056</v>
+        <v>-0.406504065040655</v>
       </c>
       <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <v>-0.4032258064516172</v>
+        <v>0.0567413667111164</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
       </c>
       <c r="AH9">
-        <v>0.2288329519450653</v>
+        <v>-0.403225806451617</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <v>0.228832951945065</v>
       </c>
       <c r="AJ9">
-        <v>0.08278341307627635</v>
+        <v>0.0827968265835726</v>
       </c>
       <c r="AK9">
         <v>0</v>
       </c>
       <c r="AL9">
-        <v>0.06989218757427608</v>
+        <v>0.0698987198358996</v>
       </c>
       <c r="AM9">
         <v>0</v>
@@ -1702,13 +1702,13 @@
         <v>0</v>
       </c>
       <c r="AO9">
-        <v>0.05458321699054506</v>
+        <v>0.0545978898018857</v>
       </c>
       <c r="AP9">
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>-0.4115226337448697</v>
+        <v>-0.41152263374487</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -1722,43 +1722,43 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.0768184580361615</v>
+        <v>0.0767745106672295</v>
       </c>
       <c r="E10">
-        <v>-0.1434720229555296</v>
+        <v>-0.14347202295553</v>
       </c>
       <c r="F10">
-        <v>-0.6097919972567987</v>
+        <v>-0.609749656055338</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>-0.4065040650406548</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0.05266852229966082</v>
+        <v>-0.406504065040655</v>
       </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>-0.4032258064516172</v>
+        <v>0.052674191159765</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>0.2288329519450653</v>
+        <v>-0.403225806451617</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.228832951945065</v>
       </c>
       <c r="O10">
-        <v>0.07668917767998105</v>
+        <v>0.0766971558747176</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>-9.020364910921192</v>
+        <v>-9.02036669539881</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1767,13 +1767,13 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>0.05075293809091167</v>
+        <v>0.0507595759579253</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10">
-        <v>-0.8230452674897143</v>
+        <v>-0.823045267489714</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1782,13 +1782,13 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>-0.09401855861538971</v>
+        <v>-0.0940570259060667</v>
       </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0.7414934654816809</v>
+        <v>0.741539849610118</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -1797,12 +1797,12 @@
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>-0.06456243178414206</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
+        <v>-0.0645550330709693</v>
+      </c>
+      <c r="AF10">
         <v>0</v>
       </c>
       <c r="AH10">
@@ -1812,13 +1812,13 @@
         <v>0</v>
       </c>
       <c r="AJ10">
-        <v>-0.09382830661142595</v>
+        <v>-0.0938176651660651</v>
       </c>
       <c r="AK10">
         <v>0</v>
       </c>
       <c r="AL10">
-        <v>11.00373724361165</v>
+        <v>11.0037359296815</v>
       </c>
       <c r="AM10">
         <v>0</v>
@@ -1827,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="AO10">
-        <v>-0.06221716219906433</v>
+        <v>-0.0622116079348764</v>
       </c>
       <c r="AP10">
         <v>0</v>
       </c>
       <c r="AQ10">
-        <v>0.4115226337448445</v>
+        <v>0.411522633744845</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -1841,124 +1841,124 @@
         <v>51</v>
       </c>
       <c r="B11">
-        <v>-1.459143968871586</v>
+        <v>-1.45914396887159</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>39.05748969846252</v>
+        <v>39.0574405504174</v>
       </c>
       <c r="E11">
         <v>-2.91136681406078</v>
       </c>
       <c r="F11">
-        <v>271.3853152335996</v>
+        <v>271.385484997489</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>-7.205391820035612</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>15.47725571835285</v>
+        <v>-7.20539182003561</v>
       </c>
       <c r="J11">
-        <v>-1.434559153734826</v>
-      </c>
-      <c r="L11">
-        <v>-5.908262888487718</v>
+        <v>15.4772649354426</v>
+      </c>
+      <c r="K11">
+        <v>-1.43455915373483</v>
       </c>
       <c r="M11">
-        <v>1.712971643237437</v>
+        <v>-5.90826288848772</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1.71297164323744</v>
       </c>
       <c r="O11">
-        <v>14.62923075441406</v>
+        <v>14.6292407854785</v>
       </c>
       <c r="P11">
-        <v>-1.434559153734826</v>
+        <v>-1.43455915373483</v>
       </c>
       <c r="Q11">
-        <v>27.80318780730525</v>
+        <v>27.8031881060092</v>
       </c>
       <c r="R11">
-        <v>-1.468974461292888</v>
+        <v>-1.46897446129289</v>
       </c>
       <c r="S11">
-        <v>-1.434559153734826</v>
+        <v>-1.43455915373483</v>
       </c>
       <c r="T11">
-        <v>28.31278596615858</v>
+        <v>28.312798185325</v>
       </c>
       <c r="U11">
-        <v>-1.459143968871586</v>
+        <v>-1.45914396887159</v>
       </c>
       <c r="V11">
-        <v>-11.87417846772167</v>
+        <v>-11.8741784677217</v>
       </c>
       <c r="W11">
-        <v>1.092487279257695</v>
+        <v>1.0924872792577</v>
       </c>
       <c r="X11">
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>-84.12648646070483</v>
+        <v>-84.1264926086068</v>
       </c>
       <c r="Z11">
-        <v>117.4852638333618</v>
+        <v>117.485263833362</v>
       </c>
       <c r="AA11">
-        <v>-92.82151620635091</v>
+        <v>-92.8215150499036</v>
       </c>
       <c r="AB11">
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>4.631222660774323</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <v>-79.53611254887946</v>
+        <v>4.63122266077432</v>
       </c>
       <c r="AE11">
-        <v>1.012923506811042</v>
-      </c>
-      <c r="AG11">
-        <v>4.585787266318652</v>
+        <v>-79.5361202625606</v>
+      </c>
+      <c r="AF11">
+        <v>1.01292350681104</v>
       </c>
       <c r="AH11">
-        <v>-21.90580077135845</v>
+        <v>4.58578726631865</v>
       </c>
       <c r="AI11">
-        <v>0</v>
+        <v>-21.9058007713585</v>
       </c>
       <c r="AJ11">
-        <v>-79.92749888132143</v>
+        <v>-79.927503961319</v>
       </c>
       <c r="AK11">
-        <v>0.9979541939024963</v>
+        <v>0.997954193902496</v>
       </c>
       <c r="AL11">
-        <v>-81.09301352336595</v>
+        <v>-81.0930237129139</v>
       </c>
       <c r="AM11">
-        <v>0.9776536312849128</v>
+        <v>0.977653631284913</v>
       </c>
       <c r="AN11">
-        <v>1.012923506811042</v>
+        <v>1.01292350681104</v>
       </c>
       <c r="AO11">
-        <v>-81.10525999105809</v>
+        <v>-81.1052654695486</v>
       </c>
       <c r="AP11">
-        <v>0.9877282250823072</v>
+        <v>0.987728225082307</v>
       </c>
       <c r="AQ11">
-        <v>10.44288487042445</v>
+        <v>10.4428848704245</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -1966,124 +1966,124 @@
         <v>52</v>
       </c>
       <c r="B12">
-        <v>-1.913099870298311</v>
+        <v>-1.91309987029831</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>46.11280032147779</v>
+        <v>46.1127495919463</v>
       </c>
       <c r="E12">
-        <v>-2.754498664241726</v>
+        <v>-2.75449866424173</v>
       </c>
       <c r="F12">
-        <v>208.1748489317904</v>
+        <v>208.174967343224</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>-7.60458757798004</v>
       </c>
-      <c r="I12">
-        <v>13.10636180681189</v>
-      </c>
       <c r="J12">
-        <v>-1.888628311960471</v>
-      </c>
-      <c r="L12">
-        <v>-5.883784836864028</v>
+        <v>13.1063692878842</v>
+      </c>
+      <c r="K12">
+        <v>-1.88862831196047</v>
       </c>
       <c r="M12">
-        <v>1.950413223140484</v>
+        <v>-5.88378483686403</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1.95041322314048</v>
       </c>
       <c r="O12">
-        <v>11.96942501811966</v>
+        <v>11.9694365444678</v>
       </c>
       <c r="P12">
-        <v>-1.888628311960471</v>
+        <v>-1.88862831196047</v>
       </c>
       <c r="Q12">
-        <v>23.59541917270496</v>
+        <v>23.5954143372622</v>
       </c>
       <c r="R12">
-        <v>-1.922885075818034</v>
+        <v>-1.92288507581803</v>
       </c>
       <c r="S12">
-        <v>-1.888628311960471</v>
+        <v>-1.88862831196047</v>
       </c>
       <c r="T12">
-        <v>12.72166498966774</v>
+        <v>12.7216745561315</v>
       </c>
       <c r="U12">
-        <v>-1.945525291828787</v>
+        <v>-1.94552529182879</v>
       </c>
       <c r="V12">
-        <v>-11.46632342591938</v>
+        <v>-11.4663234259194</v>
       </c>
       <c r="W12">
-        <v>0.6385313778309865</v>
+        <v>0.638531377830986</v>
       </c>
       <c r="X12">
         <v>0</v>
       </c>
       <c r="Y12">
-        <v>-75.49970518233181</v>
+        <v>-75.4995249763417</v>
       </c>
       <c r="Z12">
-        <v>116.5425559345325</v>
+        <v>116.542555934533</v>
       </c>
       <c r="AA12">
-        <v>-87.0536720721456</v>
+        <v>-87.0536672894672</v>
       </c>
       <c r="AB12">
         <v>0</v>
       </c>
       <c r="AC12">
-        <v>5.067186088527547</v>
+        <v>0</v>
       </c>
       <c r="AD12">
-        <v>-64.84665032515153</v>
+        <v>5.06718608852755</v>
       </c>
       <c r="AE12">
+        <v>-64.8466565198912</v>
+      </c>
+      <c r="AF12">
         <v>0.558854348585398</v>
       </c>
-      <c r="AG12">
-        <v>5.860009635962302</v>
-      </c>
       <c r="AH12">
-        <v>-17.91544001965509</v>
+        <v>5.8600096359623</v>
       </c>
       <c r="AI12">
-        <v>0</v>
+        <v>-17.9154400196551</v>
       </c>
       <c r="AJ12">
-        <v>-65.79973653071679</v>
+        <v>-65.7997403313872</v>
       </c>
       <c r="AK12">
-        <v>0.5763185469786958</v>
+        <v>0.576318546978696</v>
       </c>
       <c r="AL12">
-        <v>-67.88742112786437</v>
+        <v>-67.8874307024365</v>
       </c>
       <c r="AM12">
-        <v>0.5586592178770931</v>
+        <v>0.558659217877093</v>
       </c>
       <c r="AN12">
-        <v>0.5937827453719935</v>
+        <v>0.593782745371993</v>
       </c>
       <c r="AO12">
-        <v>-64.33326376297693</v>
+        <v>-64.3332702933262</v>
       </c>
       <c r="AP12">
-        <v>0.5686920083807223</v>
+        <v>0.568692008380722</v>
       </c>
       <c r="AQ12">
-        <v>10.49382716049383</v>
+        <v>10.4938271604938</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -2091,124 +2091,124 @@
         <v>53</v>
       </c>
       <c r="B13">
-        <v>-3.177691309987027</v>
+        <v>-3.17769130998703</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>-85.08291833691423</v>
+        <v>-85.0828781386225</v>
       </c>
       <c r="E13">
-        <v>0.1983943280776284</v>
+        <v>0.198394328077628</v>
       </c>
       <c r="F13">
-        <v>-93.60481929059543</v>
+        <v>-93.6047913202512</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>7.561694714912536</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>-82.88865887691418</v>
+        <v>7.56169471491254</v>
       </c>
       <c r="J13">
-        <v>-3.250835786637386</v>
-      </c>
-      <c r="L13">
-        <v>8.778133991709851</v>
+        <v>-82.8885964781546</v>
+      </c>
+      <c r="K13">
+        <v>-3.25083578663739</v>
       </c>
       <c r="M13">
-        <v>-24.37017293517728</v>
+        <v>8.77813399170985</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>-24.3701729351773</v>
       </c>
       <c r="O13">
-        <v>-82.3497359191029</v>
+        <v>-82.3496746002573</v>
       </c>
       <c r="P13">
-        <v>-3.348136320542884</v>
+        <v>-3.34813632054288</v>
       </c>
       <c r="Q13">
-        <v>-82.21539484614368</v>
+        <v>-82.2153365897888</v>
       </c>
       <c r="R13">
-        <v>-3.284616919393456</v>
+        <v>-3.28461691939346</v>
       </c>
       <c r="S13">
-        <v>-3.250835786637386</v>
+        <v>-3.25083578663739</v>
       </c>
       <c r="T13">
-        <v>-82.21927219222415</v>
+        <v>-82.2192137546708</v>
       </c>
       <c r="U13">
         <v>-3.27496757457847</v>
       </c>
       <c r="V13">
-        <v>13.60813524183732</v>
+        <v>13.6081352418373</v>
       </c>
       <c r="W13">
-        <v>3.013069939139984</v>
+        <v>3.01306993913998</v>
       </c>
       <c r="X13">
         <v>0</v>
       </c>
       <c r="Y13">
-        <v>41.40780917939578</v>
+        <v>41.4077659018285</v>
       </c>
       <c r="Z13">
-        <v>-5.316246382802818</v>
+        <v>-5.31624638280282</v>
       </c>
       <c r="AA13">
-        <v>359.1246005251724</v>
+        <v>359.124859612872</v>
       </c>
       <c r="AB13">
         <v>0</v>
       </c>
       <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
         <v>-11.6284966239493</v>
       </c>
-      <c r="AD13">
-        <v>26.60622561032265</v>
-      </c>
       <c r="AE13">
-        <v>3.038770520433126</v>
-      </c>
-      <c r="AG13">
-        <v>-11.16716785128487</v>
+        <v>26.6062359652646</v>
+      </c>
+      <c r="AF13">
+        <v>3.03877052043313</v>
       </c>
       <c r="AH13">
-        <v>3.739252331270317</v>
+        <v>-11.1671678512849</v>
       </c>
       <c r="AI13">
-        <v>0</v>
+        <v>3.73925233127032</v>
       </c>
       <c r="AJ13">
-        <v>18.57903790454727</v>
+        <v>18.57905341666</v>
       </c>
       <c r="AK13">
-        <v>3.038770520433126</v>
+        <v>3.03877052043313</v>
       </c>
       <c r="AL13">
-        <v>29.71320473567199</v>
+        <v>29.7132068607616</v>
       </c>
       <c r="AM13">
-        <v>3.002793296089391</v>
+        <v>3.00279329608939</v>
       </c>
       <c r="AN13">
-        <v>3.038770520433126</v>
+        <v>3.03877052043313</v>
       </c>
       <c r="AO13">
-        <v>30.33696287062384</v>
+        <v>30.3369789301831</v>
       </c>
       <c r="AP13">
-        <v>3.013069939139984</v>
+        <v>3.01306993913998</v>
       </c>
       <c r="AQ13">
-        <v>-17.29817953546768</v>
+        <v>-17.2981795354677</v>
       </c>
     </row>
     <row r="14" spans="1:43">
@@ -2216,124 +2216,124 @@
         <v>54</v>
       </c>
       <c r="B14">
-        <v>-3.404669260700389</v>
+        <v>-3.40466926070039</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>-78.11733279954723</v>
+        <v>-78.117355990609</v>
       </c>
       <c r="E14">
-        <v>-1.830580106870358</v>
+        <v>-1.83058010687036</v>
       </c>
       <c r="F14">
-        <v>-90.16318870227413</v>
+        <v>-90.1631943159874</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1.076277512154768</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>-73.43162110263431</v>
+        <v>1.07627751215477</v>
       </c>
       <c r="J14">
-        <v>-3.510303877052035</v>
-      </c>
-      <c r="L14">
+        <v>-73.4316331996608</v>
+      </c>
+      <c r="K14">
+        <v>-3.51030387705204</v>
+      </c>
+      <c r="M14">
         <v>2.38432345642972</v>
       </c>
-      <c r="M14">
-        <v>-17.55929953611206</v>
-      </c>
       <c r="N14">
-        <v>0</v>
+        <v>-17.5592995361121</v>
       </c>
       <c r="O14">
-        <v>-74.16517026425947</v>
+        <v>-74.1651808014384</v>
       </c>
       <c r="P14">
-        <v>-3.542737388353878</v>
+        <v>-3.54273738835388</v>
       </c>
       <c r="Q14">
-        <v>-74.0664254424787</v>
+        <v>-74.06644062552</v>
       </c>
       <c r="R14">
-        <v>-3.511572226656013</v>
+        <v>-3.51157222665601</v>
       </c>
       <c r="S14">
-        <v>-3.477870365750192</v>
+        <v>-3.47787036575019</v>
       </c>
       <c r="T14">
-        <v>-74.06338196711832</v>
+        <v>-74.063390836141</v>
       </c>
       <c r="U14">
-        <v>-3.501945525291816</v>
+        <v>-3.50194552529182</v>
       </c>
       <c r="V14">
-        <v>7.051367146946593</v>
+        <v>7.05136714694659</v>
       </c>
       <c r="W14">
-        <v>2.559114037713258</v>
+        <v>2.55911403771326</v>
       </c>
       <c r="X14">
         <v>0</v>
       </c>
       <c r="Y14">
-        <v>41.20347550304685</v>
+        <v>41.2034029904579</v>
       </c>
       <c r="Z14">
-        <v>-2.133328384899606</v>
+        <v>-2.13332838489961</v>
       </c>
       <c r="AA14">
-        <v>315.9641413237547</v>
+        <v>315.96416058052</v>
       </c>
       <c r="AB14">
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>-0.9345302850372788</v>
+        <v>0</v>
       </c>
       <c r="AD14">
-        <v>19.72411969127052</v>
+        <v>-0.934530285037279</v>
       </c>
       <c r="AE14">
-        <v>2.619629758994078</v>
-      </c>
-      <c r="AG14">
-        <v>-1.766892114451344</v>
+        <v>19.724117230946</v>
+      </c>
+      <c r="AF14">
+        <v>2.61962975899408</v>
       </c>
       <c r="AH14">
-        <v>-0.7102737079853911</v>
+        <v>-1.76689211445134</v>
       </c>
       <c r="AI14">
-        <v>0</v>
+        <v>-0.710273707985391</v>
       </c>
       <c r="AJ14">
-        <v>19.1751833827104</v>
+        <v>19.175186953066</v>
       </c>
       <c r="AK14">
-        <v>2.619629758994078</v>
+        <v>2.61962975899408</v>
       </c>
       <c r="AL14">
-        <v>29.05808506697943</v>
+        <v>29.0580633347405</v>
       </c>
       <c r="AM14">
-        <v>2.583798882681571</v>
+        <v>2.58379888268157</v>
       </c>
       <c r="AN14">
-        <v>2.584701362207482</v>
+        <v>2.58470136220748</v>
       </c>
       <c r="AO14">
-        <v>29.53765334780476</v>
+        <v>29.5376502027646</v>
       </c>
       <c r="AP14">
-        <v>2.594033722438399</v>
+        <v>2.5940337224384</v>
       </c>
       <c r="AQ14">
-        <v>-7.733768107416086</v>
+        <v>-7.73376810741609</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -2341,64 +2341,64 @@
         <v>55</v>
       </c>
       <c r="B15">
-        <v>-0.06485084306096763</v>
+        <v>-0.0648508430609676</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>-0.5112056872780701</v>
+        <v>-0.511247191761796</v>
       </c>
       <c r="E15">
-        <v>-0.07366669057031927</v>
+        <v>-0.0736666905703193</v>
       </c>
       <c r="F15">
-        <v>-1.351854622641086</v>
+        <v>-1.35182390346906</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>-0.3717054990256506</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>-0.2988669303614323</v>
+        <v>-0.371705499025651</v>
       </c>
       <c r="J15">
-        <v>-0.06985679357317474</v>
-      </c>
-      <c r="L15">
-        <v>0.06990562740300899</v>
+        <v>-0.298863457164252</v>
+      </c>
+      <c r="K15">
+        <v>-0.0698567935731747</v>
       </c>
       <c r="M15">
-        <v>0.06489292667099618</v>
+        <v>0.069905627403009</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>0.0648929266709962</v>
       </c>
       <c r="O15">
-        <v>-0.3633193948936104</v>
+        <v>-0.363312818176065</v>
       </c>
       <c r="P15">
-        <v>-0.06985679357317474</v>
+        <v>-0.0698567935731747</v>
       </c>
       <c r="Q15">
-        <v>-0.3464688083799473</v>
+        <v>-0.34647315026277</v>
       </c>
       <c r="R15">
-        <v>-0.06983240223463663</v>
+        <v>-0.0698324022346366</v>
       </c>
       <c r="S15">
-        <v>-0.03492839678657931</v>
+        <v>-0.0349283967865793</v>
       </c>
       <c r="T15">
-        <v>-0.332180265826809</v>
+        <v>-0.332176341499489</v>
       </c>
       <c r="U15">
-        <v>-0.06485084306096763</v>
+        <v>-0.0648508430609676</v>
       </c>
       <c r="V15">
-        <v>-0.3419290087509778</v>
+        <v>-0.341929008750978</v>
       </c>
       <c r="W15">
         <v>0.0648508430609515</v>
@@ -2407,58 +2407,58 @@
         <v>0</v>
       </c>
       <c r="Y15">
-        <v>0.5167516217193471</v>
+        <v>0.516685231961735</v>
       </c>
       <c r="Z15">
         <v>-0.069808027923219</v>
       </c>
       <c r="AA15">
-        <v>1.385381135567624</v>
+        <v>1.38546955930542</v>
       </c>
       <c r="AB15">
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>-0.8822486130620579</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <v>0.2999536966507372</v>
+        <v>-0.882248613062058</v>
       </c>
       <c r="AE15">
-        <v>0.06985679357319088</v>
-      </c>
-      <c r="AG15">
-        <v>-0.4727523503912605</v>
+        <v>0.299969219882882</v>
+      </c>
+      <c r="AF15">
+        <v>0.0698567935731909</v>
       </c>
       <c r="AH15">
-        <v>0.3925604820470683</v>
+        <v>-0.47275235039126</v>
       </c>
       <c r="AI15">
-        <v>0</v>
+        <v>0.392560482047068</v>
       </c>
       <c r="AJ15">
-        <v>0.3652686736153885</v>
+        <v>0.365287953804437</v>
       </c>
       <c r="AK15">
-        <v>0.06985679357319088</v>
+        <v>0.0698567935731909</v>
       </c>
       <c r="AL15">
-        <v>0.3490970548034841</v>
+        <v>0.349103027315683</v>
       </c>
       <c r="AM15">
-        <v>0.06983240223463663</v>
+        <v>0.0698324022346366</v>
       </c>
       <c r="AN15">
-        <v>0.06985679357319088</v>
+        <v>0.0698567935731909</v>
       </c>
       <c r="AO15">
-        <v>0.3342870355503912</v>
+        <v>0.334305229354675</v>
       </c>
       <c r="AP15">
         <v>0.0648508430609515</v>
       </c>
       <c r="AQ15">
-        <v>-0.8922545869122487</v>
+        <v>-0.892254586912249</v>
       </c>
     </row>
     <row r="16" spans="1:43">
@@ -2466,121 +2466,121 @@
         <v>56</v>
       </c>
       <c r="B16">
-        <v>-0.2269779507133625</v>
+        <v>-0.226977950713362</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>-52.82603465769598</v>
+        <v>-52.8261064453465</v>
       </c>
       <c r="E16">
-        <v>0.4240842037553818</v>
+        <v>0.424084203755382</v>
       </c>
       <c r="F16">
-        <v>-72.91464942187696</v>
+        <v>-72.9146782252752</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>4.320102024549668</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>-40.71563329945301</v>
+        <v>4.32010202454967</v>
       </c>
       <c r="J16">
-        <v>-0.2444987775061035</v>
-      </c>
-      <c r="L16">
-        <v>4.691453194180896</v>
+        <v>-40.7156919084894</v>
+      </c>
+      <c r="K16">
+        <v>-0.244498777506104</v>
       </c>
       <c r="M16">
-        <v>-9.176000577102275</v>
+        <v>4.6914531941809</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>-9.17600057710228</v>
       </c>
       <c r="O16">
-        <v>-38.8102378744737</v>
+        <v>-38.8103020656931</v>
       </c>
       <c r="P16">
         <v>-0.279427174292699</v>
       </c>
       <c r="Q16">
-        <v>-40.87391711586721</v>
+        <v>-40.8739779410984</v>
       </c>
       <c r="R16">
-        <v>-0.2793296089385465</v>
+        <v>-0.279329608938547</v>
       </c>
       <c r="S16">
-        <v>-0.2444987775061035</v>
+        <v>-0.244498777506104</v>
       </c>
       <c r="T16">
-        <v>-40.89633958960398</v>
+        <v>-40.8963956098487</v>
       </c>
       <c r="U16">
-        <v>-0.2693804250224474</v>
+        <v>-0.269380425022447</v>
       </c>
       <c r="V16">
         <v>7.2955931343731</v>
       </c>
       <c r="W16">
-        <v>-1.264591439688715</v>
+        <v>-1.26459143968872</v>
       </c>
       <c r="X16">
         <v>0</v>
       </c>
       <c r="Y16">
-        <v>32.51686713077937</v>
+        <v>32.5168134664928</v>
       </c>
       <c r="Z16">
-        <v>-0.6330274880217924</v>
+        <v>-0.633027488021792</v>
       </c>
       <c r="AA16">
-        <v>147.3275787127248</v>
+        <v>147.327620985035</v>
       </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>-3.683767872161495</v>
+        <v>0</v>
       </c>
       <c r="AD16">
-        <v>10.43185498767948</v>
+        <v>-3.68376787216149</v>
       </c>
       <c r="AE16">
-        <v>-1.239958085923848</v>
-      </c>
-      <c r="AG16">
-        <v>-3.643934856393135</v>
+        <v>10.4318581140238</v>
+      </c>
+      <c r="AF16">
+        <v>-1.23995808592385</v>
       </c>
       <c r="AH16">
-        <v>-2.427432900091319</v>
+        <v>-3.64393485639313</v>
       </c>
       <c r="AI16">
-        <v>0</v>
+        <v>-2.42743290009132</v>
       </c>
       <c r="AJ16">
-        <v>2.813920339740742</v>
+        <v>2.81392693804595</v>
       </c>
       <c r="AK16">
-        <v>-1.239958085923848</v>
+        <v>-1.23995808592385</v>
       </c>
       <c r="AL16">
-        <v>11.14812625397123</v>
+        <v>11.1481202397525</v>
       </c>
       <c r="AM16">
-        <v>-1.274441340782122</v>
+        <v>-1.27444134078212</v>
       </c>
       <c r="AN16">
-        <v>-1.239958085923848</v>
+        <v>-1.23995808592385</v>
       </c>
       <c r="AO16">
-        <v>11.46923616239787</v>
+        <v>11.4692419462952</v>
       </c>
       <c r="AP16">
-        <v>-1.232166018158224</v>
+        <v>-1.23216601815822</v>
       </c>
       <c r="AQ16">
         <v>-6.62897104787272</v>
@@ -2597,115 +2597,115 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>-53.12441376638701</v>
+        <v>-53.1244252931314</v>
       </c>
       <c r="E17">
-        <v>0.4592713390755597</v>
+        <v>0.45927133907556</v>
       </c>
       <c r="F17">
-        <v>-73.1112831044243</v>
+        <v>-73.1112781387911</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>4.393206510901826</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>-41.04003855029429</v>
+        <v>4.39320651090183</v>
       </c>
       <c r="J17">
+        <v>-41.0400463055168</v>
+      </c>
+      <c r="K17">
         <v>-0.279427174292699</v>
       </c>
-      <c r="L17">
-        <v>3.919411332693072</v>
-      </c>
       <c r="M17">
-        <v>-8.887425350226044</v>
+        <v>3.91941133269307</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>-8.88742535022604</v>
       </c>
       <c r="O17">
-        <v>-39.15539720137284</v>
+        <v>-39.1553994352943</v>
       </c>
       <c r="P17">
-        <v>-0.3143555710792783</v>
+        <v>-0.314355571079278</v>
       </c>
       <c r="Q17">
-        <v>-41.20077776064404</v>
+        <v>-41.200784927978</v>
       </c>
       <c r="R17">
-        <v>-0.3142458100558729</v>
+        <v>-0.314245810055873</v>
       </c>
       <c r="S17">
-        <v>-0.3143555710792783</v>
+        <v>-0.314355571079278</v>
       </c>
       <c r="T17">
-        <v>-41.22396455390175</v>
+        <v>-41.2239711446661</v>
       </c>
       <c r="U17">
-        <v>-0.3043001097475875</v>
+        <v>-0.304300109747588</v>
       </c>
       <c r="V17">
-        <v>7.745994681196089</v>
+        <v>7.74599468119609</v>
       </c>
       <c r="W17">
-        <v>-1.264591439688715</v>
+        <v>-1.26459143968872</v>
       </c>
       <c r="X17">
         <v>0</v>
       </c>
       <c r="Y17">
-        <v>32.51830294431981</v>
+        <v>32.518248258556</v>
       </c>
       <c r="Z17">
-        <v>-0.7958435728795371</v>
+        <v>-0.795843572879537</v>
       </c>
       <c r="AA17">
-        <v>147.3275031422349</v>
+        <v>147.327560483566</v>
       </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>-3.715388434252056</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <v>10.43238664065442</v>
+        <v>-3.71538843425206</v>
       </c>
       <c r="AE17">
-        <v>-1.239958085923848</v>
-      </c>
-      <c r="AG17">
-        <v>-4.052223268018597</v>
+        <v>10.432389769445</v>
+      </c>
+      <c r="AF17">
+        <v>-1.23995808592385</v>
       </c>
       <c r="AH17">
-        <v>-2.195669082751856</v>
+        <v>-4.0522232680186</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <v>-2.19566908275186</v>
       </c>
       <c r="AJ17">
-        <v>2.814501009554768</v>
+        <v>2.81450693941465</v>
       </c>
       <c r="AK17">
         <v>-1.22249388753055</v>
       </c>
       <c r="AL17">
-        <v>11.1487402874816</v>
+        <v>11.148730832858</v>
       </c>
       <c r="AM17">
-        <v>-1.274441340782122</v>
+        <v>-1.27444134078212</v>
       </c>
       <c r="AN17">
-        <v>-1.207524574622005</v>
+        <v>-1.207524574622</v>
       </c>
       <c r="AO17">
-        <v>11.46945463845802</v>
+        <v>11.4694590014297</v>
       </c>
       <c r="AP17">
-        <v>-1.232166018158224</v>
+        <v>-1.23216601815822</v>
       </c>
       <c r="AQ17">
         <v>-6.21213609719357</v>
@@ -2722,58 +2722,58 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>-9.117779304567021</v>
+        <v>-9.11780908627742</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>-0.09009784518381142</v>
+        <v>-0.0900762025121434</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>-0.441278330381083</v>
       </c>
-      <c r="I18">
-        <v>-0.01317145109170965</v>
-      </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+        <v>-0.0131681267125255</v>
+      </c>
+      <c r="K18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0.2288329519450653</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>0.228832951945065</v>
       </c>
       <c r="O18">
-        <v>-0.004087897717774873</v>
+        <v>-0.0040809176804166</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>-0.01244922864683681</v>
+        <v>-0.0124522427211662</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.03492839678659544</v>
+        <v>0.0349283967865954</v>
       </c>
       <c r="T18">
-        <v>-0.01262547523819337</v>
+        <v>-0.0126197810088795</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18">
-        <v>-0.4115226337448697</v>
+        <v>-0.41152263374487</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2782,13 +2782,13 @@
         <v>0</v>
       </c>
       <c r="Y18">
-        <v>11.15105570297653</v>
+        <v>11.1510107741499</v>
       </c>
       <c r="Z18">
         <v>0.143472022955512</v>
       </c>
       <c r="AA18">
-        <v>0.1099552975731667</v>
+        <v>0.109990194743762</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -2797,12 +2797,12 @@
         <v>0</v>
       </c>
       <c r="AD18">
-        <v>0.01585645798794538</v>
+        <v>0</v>
       </c>
       <c r="AE18">
-        <v>0</v>
-      </c>
-      <c r="AG18">
+        <v>0.0158600766644008</v>
+      </c>
+      <c r="AF18">
         <v>0</v>
       </c>
       <c r="AH18">
@@ -2812,13 +2812,13 @@
         <v>0</v>
       </c>
       <c r="AJ18">
-        <v>0.004870892792509566</v>
+        <v>0.00487875429939443</v>
       </c>
       <c r="AK18">
         <v>0</v>
       </c>
       <c r="AL18">
-        <v>0.01512832241114821</v>
+        <v>0.0151283443674231</v>
       </c>
       <c r="AM18">
         <v>0</v>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="AO18">
-        <v>0.0153653177622399</v>
+        <v>0.0153683975682669</v>
       </c>
       <c r="AP18">
         <v>0</v>

</xml_diff>